<commit_message>
add 6 mm lab and 11 aln lab
</commit_message>
<xml_diff>
--- a/2020-2021/ALN/lab3/cеть172.xlsx
+++ b/2020-2021/ALN/lab3/cеть172.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsok\work\2020-2021\ALN\lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09483648-CD1C-41F0-905A-6FE40AB40D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9B4B43-E02E-4525-B65F-810960019654}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VLAN" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>№ VLAN</t>
   </si>
@@ -83,141 +83,48 @@
     <t>IP-адреса</t>
   </si>
   <si>
-    <t>172.16.0.0/12</t>
-  </si>
-  <si>
     <t>Вся сеть</t>
   </si>
   <si>
-    <t>172.16.0.0/24</t>
-  </si>
-  <si>
-    <t>172.16.0.1/24</t>
-  </si>
-  <si>
     <t>Шлюз</t>
   </si>
   <si>
-    <t>172.16.0.2/24</t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
-    <t>172.16.0.3/24</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
-    <t>172.16.0.4/24</t>
-  </si>
-  <si>
     <t>Mail</t>
   </si>
   <si>
-    <t>172.16.0.5/24</t>
-  </si>
-  <si>
     <t>Dns</t>
   </si>
   <si>
-    <t>172.16.0.6-172.16.0.254</t>
-  </si>
-  <si>
-    <t>172.16.1.0/24</t>
-  </si>
-  <si>
     <t>Управление</t>
   </si>
   <si>
-    <t>172.16.1.1/24</t>
-  </si>
-  <si>
-    <t>172.16.1.2/24</t>
-  </si>
-  <si>
     <t>msk-dosnkaya-saloginov-sw1</t>
   </si>
   <si>
-    <t>172.16.1.3/24</t>
-  </si>
-  <si>
     <t>msk-dosnkaya-saloginov-sw2</t>
   </si>
   <si>
-    <t>172.16.1.4/24</t>
-  </si>
-  <si>
     <t>msk-dosnkaya-saloginov-sw3</t>
   </si>
   <si>
-    <t>172.16.1.5/24</t>
-  </si>
-  <si>
     <t>msk-dosnkaya-saloginov-sw4</t>
   </si>
   <si>
-    <t>172.16.1.6/24</t>
-  </si>
-  <si>
     <t>msk-pavlovskaya-saloginov-sw1</t>
   </si>
   <si>
-    <t>172.16.1.7-172.16.1.254</t>
-  </si>
-  <si>
-    <t>172.16.2.0/24</t>
-  </si>
-  <si>
     <t>Сеть Point-to-Point</t>
   </si>
   <si>
-    <t>172.16.2.1/24</t>
-  </si>
-  <si>
-    <t>172.16.2.2-172.16.2.254</t>
-  </si>
-  <si>
-    <t>172.16.3.0/24</t>
-  </si>
-  <si>
-    <t>172.16.3.1/24</t>
-  </si>
-  <si>
-    <t>172.16.3.2-172.16.3.254</t>
-  </si>
-  <si>
     <t>Пул для пользователей</t>
   </si>
   <si>
-    <t>172.16.4.0/24</t>
-  </si>
-  <si>
-    <t>172.16.4.1/24</t>
-  </si>
-  <si>
-    <t>172.16.4.2-172.16.4.254</t>
-  </si>
-  <si>
-    <t>172.16.5.0/24</t>
-  </si>
-  <si>
-    <t>172.16.5.1/24</t>
-  </si>
-  <si>
-    <t>172.16.5.2-172.16.5.254</t>
-  </si>
-  <si>
-    <t>172.16.6.0/24</t>
-  </si>
-  <si>
-    <t>172.16.6.1/24</t>
-  </si>
-  <si>
-    <t>172.16.6.2-172.16.6.254</t>
-  </si>
-  <si>
     <t>Устройство</t>
   </si>
   <si>
@@ -315,13 +222,136 @@
   </si>
   <si>
     <t>f0/20</t>
+  </si>
+  <si>
+    <t>10.128.0.0/12</t>
+  </si>
+  <si>
+    <t>10.128.0.0/24</t>
+  </si>
+  <si>
+    <t>10.128.0.1/24</t>
+  </si>
+  <si>
+    <t>10.128.0.2/24</t>
+  </si>
+  <si>
+    <t>10.128.0.3/24</t>
+  </si>
+  <si>
+    <t>10.128.0.4/24</t>
+  </si>
+  <si>
+    <t>10.128.0.5/24</t>
+  </si>
+  <si>
+    <t>10.128.0.6-10.128.0.254</t>
+  </si>
+  <si>
+    <t>10.128.1.0/24</t>
+  </si>
+  <si>
+    <t>10.128.1.1/24</t>
+  </si>
+  <si>
+    <t>10.128.1.2/24</t>
+  </si>
+  <si>
+    <t>10.128.1.3/24</t>
+  </si>
+  <si>
+    <t>10.128.1.4/24</t>
+  </si>
+  <si>
+    <t>10.128.1.5/24</t>
+  </si>
+  <si>
+    <t>10.128.1.6/24</t>
+  </si>
+  <si>
+    <t>10.128.1.7-10.128.1.254</t>
+  </si>
+  <si>
+    <t>10.128.2.0/24</t>
+  </si>
+  <si>
+    <t>10.128.2.1/24</t>
+  </si>
+  <si>
+    <t>10.128.2.2-10.128.2.254</t>
+  </si>
+  <si>
+    <t>10.128.3.0/24</t>
+  </si>
+  <si>
+    <t>10.128.3.1/24</t>
+  </si>
+  <si>
+    <t>10.128.3.2-10.128.3.254</t>
+  </si>
+  <si>
+    <t>10.128.4.0/24</t>
+  </si>
+  <si>
+    <t>10.128.4.1/24</t>
+  </si>
+  <si>
+    <t>10.128.4.2-10.128.4.254</t>
+  </si>
+  <si>
+    <t>10.128.5.0/24</t>
+  </si>
+  <si>
+    <t>10.128.5.1/24</t>
+  </si>
+  <si>
+    <t>10.128.5.2-10.128.5.254</t>
+  </si>
+  <si>
+    <t>10.128.6.0/24</t>
+  </si>
+  <si>
+    <t>10.128.6.1/24</t>
+  </si>
+  <si>
+    <t>10.128.6.2-10.128.6.254</t>
+  </si>
+  <si>
+    <t>192.0.2.1/24</t>
+  </si>
+  <si>
+    <t>192.0.2.11/24</t>
+  </si>
+  <si>
+    <t>192.0.2.12/24</t>
+  </si>
+  <si>
+    <t>192.0.2.13/24</t>
+  </si>
+  <si>
+    <t>192.0.2.14/24</t>
+  </si>
+  <si>
+    <t>Провайдер</t>
+  </si>
+  <si>
+    <t>www.yandex.ru</t>
+  </si>
+  <si>
+    <t>stud.rudn.university</t>
+  </si>
+  <si>
+    <t>esystem.pfur.ru</t>
+  </si>
+  <si>
+    <t>www.rudn.ru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +410,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -530,10 +568,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,8 +640,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1024,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FA16B1-F505-4BA4-969C-6E7842C44635}">
-  <dimension ref="B1:D39"/>
+  <dimension ref="B1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1066,16 +1130,16 @@
     </row>
     <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -1086,52 +1150,52 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" s="11"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="16" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
@@ -1140,10 +1204,10 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -1151,61 +1215,61 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="19" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="11"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D15" s="11"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D16" s="11"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D17" s="11"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="19" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D19" s="11"/>
     </row>
     <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="20" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>10</v>
@@ -1214,25 +1278,25 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" s="11"/>
     </row>
     <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="5" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>10</v>
@@ -1241,7 +1305,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>11</v>
@@ -1252,25 +1316,25 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>12</v>
@@ -1281,25 +1345,25 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="9" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="5" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>13</v>
@@ -1310,25 +1374,25 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="9" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="5" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>14</v>
@@ -1339,28 +1403,72 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="9" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="7"/>
+      <c r="B35" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="28"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="29"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="29"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="B39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="32"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C37" r:id="rId1" xr:uid="{1B2FF60C-7AE9-4EFD-BC09-ED69FE3A3147}"/>
+    <hyperlink ref="C40" r:id="rId2" xr:uid="{417E4239-2A34-4362-BE83-6DFBB15F4E1E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1369,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87736270-29AB-4905-9E23-1D98B495A803}">
   <dimension ref="A2:E30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1384,31 +1492,31 @@
   <sheetData>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
@@ -1416,14 +1524,14 @@
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1435,13 +1543,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
@@ -1449,10 +1557,10 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="11">
@@ -1462,27 +1570,27 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="11" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1494,13 +1602,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4">
@@ -1510,10 +1618,10 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="11">
@@ -1523,10 +1631,10 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D14" s="10">
         <v>3</v>
@@ -1536,10 +1644,10 @@
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D15" s="6">
         <v>3</v>
@@ -1555,13 +1663,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4">
@@ -1571,10 +1679,10 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D18" s="10">
         <v>3</v>
@@ -1584,10 +1692,10 @@
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D19" s="6">
         <v>3</v>
@@ -1603,26 +1711,26 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="10" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D22" s="10">
         <v>101</v>
@@ -1632,10 +1740,10 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="D23" s="10">
         <v>102</v>
@@ -1645,10 +1753,10 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="10" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="D24" s="10">
         <v>103</v>
@@ -1658,10 +1766,10 @@
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="D25" s="6">
         <v>104</v>
@@ -1677,26 +1785,26 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="10" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D28" s="10">
         <v>101</v>
@@ -1706,10 +1814,10 @@
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5"/>
       <c r="B29" s="6" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="D29" s="6">
         <v>104</v>

</xml_diff>